<commit_message>
created projectDetails functions based on workExperience functions. Changed functino names in workExperience to distinguish between work and project items
</commit_message>
<xml_diff>
--- a/00_resumeDetails.xlsx
+++ b/00_resumeDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bturner/personal/resume/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53321F61-79E1-5C4F-9A6F-F072793C90E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367FAB72-1BB6-2D4F-8BDC-F7091E3B8959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="34980" windowHeight="21940" xr2:uid="{E7D57012-720E-D94D-B8C8-B7C37276BDA5}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="34980" windowHeight="21940" activeTab="4" xr2:uid="{E7D57012-720E-D94D-B8C8-B7C37276BDA5}"/>
   </bookViews>
   <sheets>
     <sheet name="PersonalDetails" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="123">
   <si>
     <t>Wayfair</t>
   </si>
@@ -278,9 +278,6 @@
     <t>Data Science Blurb</t>
   </si>
   <si>
-    <t>Data Driven Problem Solving</t>
-  </si>
-  <si>
     <t>Banks, Non-Banks and Monetary Policy</t>
   </si>
   <si>
@@ -326,9 +323,6 @@
     <t>POINT 2</t>
   </si>
   <si>
-    <t>Economic Research in Finance and Innovation</t>
-  </si>
-  <si>
     <t>SecondaryTitle</t>
   </si>
   <si>
@@ -395,7 +389,16 @@
     <t>R, Python, SQL, LaTex, Stata</t>
   </si>
   <si>
-    <t>Regression and Classification Techniques</t>
+    <t>Domain knowledge in Finance and Innovation</t>
+  </si>
+  <si>
+    <t>Data driven decision making</t>
+  </si>
+  <si>
+    <t>Regression and classification techniques</t>
+  </si>
+  <si>
+    <t>ProjectYear</t>
   </si>
 </sst>
 </file>
@@ -776,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852CF9CD-6CF8-3E43-A5A2-662F5CDDF6CC}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -873,7 +876,7 @@
         <v>79</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -881,15 +884,15 @@
         <v>80</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -931,7 +934,7 @@
         <v>25</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>26</v>
@@ -971,10 +974,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" t="s">
@@ -1024,22 +1027,22 @@
         <v>30</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>27</v>
@@ -1062,13 +1065,13 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G2" s="5">
         <v>2015</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I2" s="5">
         <v>2015</v>
@@ -1094,13 +1097,13 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G3" s="5">
         <v>2017</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I3" s="5">
         <v>2017</v>
@@ -1117,7 +1120,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -1129,13 +1132,13 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G4" s="5">
         <v>2018</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I4" s="5">
         <v>2020</v>
@@ -1164,7 +1167,7 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G5" s="5">
         <v>2020</v>
@@ -1189,16 +1192,16 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G6" s="5">
         <v>2021</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I6" s="5">
         <v>2021</v>
@@ -1448,10 +1451,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CC7771-507A-6B49-A2EF-9D09725E637B}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1462,7 +1465,7 @@
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -1473,74 +1476,86 @@
         <v>35</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
         <v>83</v>
-      </c>
-      <c r="C2" t="s">
-        <v>84</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
         <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>87</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -1557,7 +1572,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1583,10 +1598,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1594,10 +1609,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1605,10 +1620,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1616,10 +1631,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1627,10 +1642,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1638,10 +1653,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1649,10 +1664,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1660,10 +1675,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1671,10 +1686,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating resume for HES application
</commit_message>
<xml_diff>
--- a/00_resumeDetails.xlsx
+++ b/00_resumeDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bturner/personal/resume/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AD2FFA-301C-624A-9641-E9A2F0688D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38611567-582F-9640-8790-242B47CFD3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="12380" windowWidth="14400" windowHeight="9660" activeTab="1" xr2:uid="{E7D57012-720E-D94D-B8C8-B7C37276BDA5}"/>
+    <workbookView xWindow="35840" yWindow="2060" windowWidth="38400" windowHeight="21140" activeTab="6" xr2:uid="{E7D57012-720E-D94D-B8C8-B7C37276BDA5}"/>
   </bookViews>
   <sheets>
     <sheet name="PersonalDetails" sheetId="7" r:id="rId1"/>
@@ -26,12 +26,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="141">
   <si>
     <t>Wayfair</t>
   </si>
@@ -339,9 +346,6 @@
     <t>Languages</t>
   </si>
   <si>
-    <t>R, Python, SQL, LaTex, Stata</t>
-  </si>
-  <si>
     <t>Domain knowledge in Finance and Innovation</t>
   </si>
   <si>
@@ -445,6 +449,18 @@
   </si>
   <si>
     <t>UK</t>
+  </si>
+  <si>
+    <t>R, Python, SQL, LaTex, Stata, PySpark</t>
+  </si>
+  <si>
+    <t>Science in Africa</t>
+  </si>
+  <si>
+    <t>AfricanScience</t>
+  </si>
+  <si>
+    <t>Pulled author information from a semi-strucutred API using Python</t>
   </si>
 </sst>
 </file>
@@ -829,7 +845,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -883,7 +899,7 @@
         <v>48</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -912,7 +928,7 @@
         <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -925,7 +941,7 @@
         <v>72</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -933,7 +949,7 @@
         <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -941,7 +957,7 @@
         <v>101</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -958,7 +974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E629FDD0-9E62-D542-A370-F2D5CF77F675}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1042,19 +1058,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" t="s">
         <v>134</v>
-      </c>
-      <c r="C4" t="s">
-        <v>135</v>
       </c>
       <c r="E4">
         <v>2016</v>
       </c>
       <c r="F4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" t="s">
         <v>136</v>
-      </c>
-      <c r="G4" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1068,7 +1084,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1228,7 +1244,7 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -1262,7 +1278,7 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F6" t="s">
         <v>88</v>
@@ -1316,7 +1332,7 @@
         <v>29</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>51</v>
@@ -1458,7 +1474,7 @@
         <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1495,7 +1511,7 @@
         <v>62</v>
       </c>
       <c r="F11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1515,7 +1531,7 @@
         <v>63</v>
       </c>
       <c r="F12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1529,7 +1545,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1564,7 +1580,7 @@
         <v>29</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>51</v>
@@ -1603,10 +1619,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CC7771-507A-6B49-A2EF-9D09725E637B}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1632,13 +1648,13 @@
         <v>75</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1646,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
         <v>74</v>
@@ -1662,7 +1678,7 @@
         <v>2019</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1686,7 +1702,7 @@
         <v>2019</v>
       </c>
       <c r="G3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1710,7 +1726,7 @@
         <v>2020</v>
       </c>
       <c r="G4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1718,7 +1734,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
         <v>82</v>
@@ -1730,8 +1746,11 @@
         <f>VLOOKUP(D5, WorkExperienceDetails!$B$1:$C$36, 2,0)</f>
         <v>Harvard Business School</v>
       </c>
+      <c r="F5">
+        <v>2021</v>
+      </c>
       <c r="G5" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1750,6 +1769,23 @@
       <c r="E6" t="str">
         <f>VLOOKUP(D6, WorkExperienceDetails!$B$1:$C$36, 2,0)</f>
         <v>Harvard Business School</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1764,10 +1800,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2875E31-AAB4-4445-B5EE-0A16F95898DC}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1796,7 +1832,7 @@
         <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1818,7 +1854,7 @@
         <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1829,7 +1865,7 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1840,7 +1876,7 @@
         <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1851,7 +1887,7 @@
         <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1862,7 +1898,7 @@
         <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1873,7 +1909,7 @@
         <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1884,7 +1920,7 @@
         <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1895,7 +1931,7 @@
         <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1903,10 +1939,21 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>128</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>